<commit_message>
feat: upload completed Sprint 1 backlog with all tasks and time logs
</commit_message>
<xml_diff>
--- a/ITSC 3155 Product Backlog (1).xlsx
+++ b/ITSC 3155 Product Backlog (1).xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Montay\OneDrive\Documents\ITSC 3155\Restaurant-API\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F763DF88-20FD-49A6-BF8A-B4FAE60B54E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="38280" yWindow="2265" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet3" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -159,18 +168,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -181,11 +188,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="13">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF374139"/>
@@ -199,6 +212,7 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -213,6 +227,7 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -227,48 +242,52 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF374139"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF374139"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF374139"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF374139"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -283,6 +302,7 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -297,6 +317,7 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -311,196 +332,183 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF374139"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF374139"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF374139"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF374139"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF374139"/>
-      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF374139"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF374139"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF374139"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF374139"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF374139"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6F8F9"/>
+          <bgColor rgb="FFF6F8F9"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF49564C"/>
           <bgColor rgb="FF49564C"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6F8F9"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="4" pivot="0" name="Sheet3-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-      <tableStyleElement size="0" type="wholeTable"/>
+    <tableStyle name="Sheet3-style" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" size="0"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E20" displayName="Project_tasks" name="Project_tasks" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Project_tasks" displayName="Project_tasks" ref="A1:E20">
   <tableColumns count="5">
-    <tableColumn name="Task" id="1"/>
-    <tableColumn name="Priority" id="2"/>
-    <tableColumn name="Status" id="3"/>
-    <tableColumn name="Due Date" id="4"/>
-    <tableColumn name="Notes" id="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Priority"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Status"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Due Date"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes"/>
   </tableColumns>
-  <tableStyleInfo name="Sheet3-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Sheet3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -690,30 +698,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.13"/>
-    <col customWidth="1" min="2" max="4" width="15.13"/>
-    <col customWidth="1" min="5" max="7" width="20.13"/>
-    <col customWidth="1" min="8" max="8" width="22.63"/>
-    <col customWidth="1" min="9" max="9" width="15.13"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,332 +742,333 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="202.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7">
-        <v>45954.0</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="6">
+        <v>45954</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:5" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="12">
-        <v>45954.0</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10">
+        <v>45954</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:5" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7">
-        <v>45954.0</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="6">
+        <v>45954</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="C5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7">
-        <v>45993.0</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="C7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:5" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7">
-        <v>45993.0</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:5" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="7">
-        <v>45993.0</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="C11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7">
-        <v>45993.0</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="C13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="7">
-        <v>45993.0</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E15" s="13" t="s">
+      <c r="C15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="7">
-        <v>45993.0</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="C16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:5" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E17" s="13" t="s">
+      <c r="C17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="7">
-        <v>45993.0</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="12">
-        <v>45993.0</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="C19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="D2:D20">
+  <dataValidations count="3">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="D2:D20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(D2))), AND(ISNUMBER(D2), LEFT(CELL("format", D2))="D"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:B20 E2:E20"/>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C20">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:B20 E2:E20" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C20" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Not started,In progress,Blocked,Completed"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: updated backlog and added sprint review
</commit_message>
<xml_diff>
--- a/ITSC 3155 Product Backlog (1).xlsx
+++ b/ITSC 3155 Product Backlog (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Montay\OneDrive\Documents\ITSC 3155\Restaurant-API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Final Project\Restaurant-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F763DF88-20FD-49A6-BF8A-B4FAE60B54E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C69C86A-C3FF-4023-9456-24FA27801F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2265" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Create a new clean repository. Invite your group member as well as Instructor team, Professor and TAs.
 Download the code skeleton and push it to the repository with a proper commit message. The rest of the group should clone the project using git clone &lt;repo_address&gt;. NOT USER STORY</t>
   </si>
@@ -53,9 +50,6 @@
     <t>Project Setup</t>
   </si>
   <si>
-    <t>Not started</t>
-  </si>
-  <si>
     <t>Create a Virtual Environment and install dependencies.
 Run the FastApi server and test the sample code. NOT USER STORY</t>
   </si>
@@ -163,6 +157,12 @@
   </si>
   <si>
     <t>Provide setup instructions and system training materials.  USER STORY</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -711,8 +711,8 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -725,7 +725,7 @@
     <col min="9" max="9" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,305 +750,305 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D2" s="6">
         <v>45954</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D3" s="10">
         <v>45954</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D4" s="6">
         <v>45954</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D5" s="10">
         <v>45993</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D6" s="6">
         <v>45993</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D7" s="10">
         <v>45993</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D8" s="6">
         <v>45993</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D9" s="10">
         <v>45993</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D10" s="6">
         <v>45993</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10">
-        <v>45993</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D12" s="6">
         <v>45993</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="10">
+        <v>45993</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="10">
-        <v>45993</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D14" s="6">
         <v>45993</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D15" s="10">
         <v>45993</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="6">
+        <v>45993</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="6">
-        <v>45993</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D17" s="10">
         <v>45993</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D18" s="6">
         <v>45993</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="D19" s="10">
         <v>45993</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>

</xml_diff>